<commit_message>
Updated the lead attenuation notebook, and fixed up the data for lead_v2 with the right shielding thicknesses
</commit_message>
<xml_diff>
--- a/data/lead_data.xlsx
+++ b/data/lead_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhafn\PHY 451\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhafn\PHY 451\PHY451-GammaRay\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443D5E3C-A3D7-45F9-8CAE-0B0DCC70F152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592138E2-FA91-45C9-86DD-E694C1A377EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12135" yWindow="3600" windowWidth="23595" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24195" yWindow="2775" windowWidth="23595" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lead_v1" sheetId="1" r:id="rId1"/>
@@ -4113,8 +4113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7993E92-AF79-4CFE-9C90-EDCE0E41B121}">
   <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="M115" sqref="M115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4135,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C2">
         <v>442</v>
@@ -4146,7 +4146,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C3">
         <v>448</v>
@@ -4157,7 +4157,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C4">
         <v>429</v>
@@ -4168,7 +4168,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C5">
         <v>411</v>
@@ -4179,7 +4179,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C6">
         <v>441</v>
@@ -4190,7 +4190,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C7">
         <v>463</v>
@@ -4201,7 +4201,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C8">
         <v>454</v>
@@ -4212,7 +4212,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C9">
         <v>481</v>
@@ -4223,7 +4223,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C10">
         <v>461</v>
@@ -4234,7 +4234,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C11">
         <v>421</v>
@@ -4245,7 +4245,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C12">
         <v>410</v>
@@ -4256,7 +4256,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C13">
         <v>427</v>
@@ -4267,7 +4267,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C14">
         <v>413</v>
@@ -4278,7 +4278,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C15">
         <v>421</v>
@@ -4289,7 +4289,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C16">
         <v>455</v>
@@ -4300,7 +4300,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C17">
         <v>456</v>
@@ -4311,7 +4311,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C18">
         <v>464</v>
@@ -4322,7 +4322,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C19">
         <v>418</v>
@@ -4333,7 +4333,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C20">
         <v>445</v>
@@ -4344,7 +4344,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C21">
         <v>427</v>
@@ -4355,7 +4355,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C22">
         <v>414</v>
@@ -4366,7 +4366,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C23">
         <v>448</v>
@@ -4377,7 +4377,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C24">
         <v>427</v>
@@ -4388,7 +4388,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C25">
         <v>442</v>
@@ -4399,7 +4399,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C26">
         <v>441</v>
@@ -4410,7 +4410,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C27">
         <v>475</v>
@@ -4421,7 +4421,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C28">
         <v>456</v>
@@ -4432,7 +4432,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C29">
         <v>477</v>
@@ -4443,7 +4443,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C30">
         <v>472</v>
@@ -4454,7 +4454,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C31">
         <v>388</v>
@@ -4465,7 +4465,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C32">
         <v>479</v>
@@ -4476,7 +4476,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C33">
         <v>427</v>
@@ -4487,7 +4487,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C34">
         <v>444</v>
@@ -4498,7 +4498,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C35">
         <v>477</v>
@@ -4509,7 +4509,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C36">
         <v>409</v>
@@ -4520,7 +4520,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C37">
         <v>454</v>
@@ -4531,7 +4531,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C38">
         <v>418</v>
@@ -4542,7 +4542,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C39">
         <v>436</v>
@@ -4553,7 +4553,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C40">
         <v>493</v>
@@ -4564,7 +4564,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C41">
         <v>448</v>
@@ -4575,7 +4575,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C42">
         <v>418</v>
@@ -4586,7 +4586,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>2.085</v>
+        <v>6.1724999999999994</v>
       </c>
       <c r="C43">
         <v>454</v>
@@ -4597,7 +4597,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C44">
         <v>300</v>
@@ -4608,7 +4608,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C45">
         <v>310</v>
@@ -4619,7 +4619,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C46">
         <v>323</v>
@@ -4630,7 +4630,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C47">
         <v>330</v>
@@ -4641,7 +4641,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C48">
         <v>331</v>
@@ -4652,7 +4652,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C49">
         <v>323</v>
@@ -4663,7 +4663,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C50">
         <v>313</v>
@@ -4674,7 +4674,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C51">
         <v>292</v>
@@ -4685,7 +4685,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C52">
         <v>283</v>
@@ -4696,7 +4696,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C53">
         <v>320</v>
@@ -4707,7 +4707,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C54">
         <v>333</v>
@@ -4718,7 +4718,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C55">
         <v>333</v>
@@ -4729,7 +4729,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C56">
         <v>319</v>
@@ -4740,7 +4740,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C57">
         <v>345</v>
@@ -4751,7 +4751,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C58">
         <v>311</v>
@@ -4762,7 +4762,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C59">
         <v>346</v>
@@ -4773,7 +4773,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C60">
         <v>296</v>
@@ -4784,7 +4784,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C61">
         <v>305</v>
@@ -4795,7 +4795,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C62">
         <v>311</v>
@@ -4806,7 +4806,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C63">
         <v>326</v>
@@ -4817,7 +4817,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C64">
         <v>301</v>
@@ -4828,7 +4828,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C65">
         <v>321</v>
@@ -4839,7 +4839,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C66">
         <v>298</v>
@@ -4850,7 +4850,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C67">
         <v>309</v>
@@ -4861,7 +4861,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C68">
         <v>332</v>
@@ -4872,7 +4872,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C69">
         <v>312</v>
@@ -4883,7 +4883,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C70">
         <v>295</v>
@@ -4894,7 +4894,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C71">
         <v>320</v>
@@ -4905,7 +4905,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>4.1749999999999998</v>
+        <v>12.614999999999998</v>
       </c>
       <c r="C72">
         <v>313</v>
@@ -4916,7 +4916,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C73">
         <v>222</v>
@@ -4927,7 +4927,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C74">
         <v>252</v>
@@ -4938,7 +4938,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C75">
         <v>213</v>
@@ -4949,7 +4949,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C76">
         <v>189</v>
@@ -4960,7 +4960,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C77">
         <v>213</v>
@@ -4971,7 +4971,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C78">
         <v>208</v>
@@ -4982,7 +4982,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C79">
         <v>246</v>
@@ -4993,7 +4993,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C80">
         <v>202</v>
@@ -5004,7 +5004,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C81">
         <v>214</v>
@@ -5015,7 +5015,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C82">
         <v>231</v>
@@ -5026,7 +5026,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C83">
         <v>261</v>
@@ -5037,7 +5037,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C84">
         <v>217</v>
@@ -5048,7 +5048,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C85">
         <v>211</v>
@@ -5059,7 +5059,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C86">
         <v>231</v>
@@ -5070,7 +5070,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C87">
         <v>222</v>
@@ -5081,7 +5081,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C88">
         <v>252</v>
@@ -5092,7 +5092,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C89">
         <v>216</v>
@@ -5103,7 +5103,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C90">
         <v>233</v>
@@ -5114,7 +5114,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C91">
         <v>228</v>
@@ -5125,7 +5125,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C92">
         <v>229</v>
@@ -5136,7 +5136,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C93">
         <v>235</v>
@@ -5147,7 +5147,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C94">
         <v>204</v>
@@ -5158,7 +5158,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C95">
         <v>214</v>
@@ -5169,7 +5169,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C96">
         <v>225</v>
@@ -5180,7 +5180,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>6.2675000000000001</v>
+        <v>26.442499999999999</v>
       </c>
       <c r="C97">
         <v>205</v>
@@ -5191,7 +5191,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C98">
         <v>131</v>
@@ -5202,7 +5202,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C99">
         <v>111</v>
@@ -5213,7 +5213,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C100">
         <v>151</v>
@@ -5224,7 +5224,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C101">
         <v>101</v>
@@ -5235,7 +5235,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C102">
         <v>130</v>
@@ -5246,7 +5246,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C103">
         <v>140</v>
@@ -5257,7 +5257,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C104">
         <v>126</v>
@@ -5268,7 +5268,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C105">
         <v>115</v>
@@ -5279,7 +5279,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C106">
         <v>131</v>
@@ -5290,7 +5290,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C107">
         <v>129</v>
@@ -5301,7 +5301,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C108">
         <v>118</v>
@@ -5312,7 +5312,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C109">
         <v>126</v>
@@ -5323,7 +5323,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C110">
         <v>141</v>
@@ -5334,7 +5334,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C111">
         <v>119</v>
@@ -5345,7 +5345,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C112">
         <v>139</v>
@@ -5356,7 +5356,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C113">
         <v>109</v>
@@ -5367,7 +5367,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C114">
         <v>117</v>
@@ -5378,7 +5378,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C115">
         <v>114</v>
@@ -5389,7 +5389,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C116">
         <v>123</v>
@@ -5400,7 +5400,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C117">
         <v>139</v>
@@ -5411,7 +5411,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C118">
         <v>109</v>
@@ -5422,7 +5422,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C119">
         <v>114</v>
@@ -5433,7 +5433,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C120">
         <v>142</v>
@@ -5444,7 +5444,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C121">
         <v>113</v>
@@ -5455,7 +5455,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C122">
         <v>139</v>
@@ -5466,7 +5466,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C123">
         <v>135</v>
@@ -5477,7 +5477,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C124">
         <v>127</v>
@@ -5488,7 +5488,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C125">
         <v>105</v>
@@ -5499,7 +5499,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C126">
         <v>119</v>
@@ -5510,7 +5510,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C127">
         <v>123</v>
@@ -5521,7 +5521,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C128">
         <v>117</v>
@@ -5532,7 +5532,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C129">
         <v>110</v>
@@ -5543,7 +5543,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C130">
         <v>109</v>
@@ -5554,7 +5554,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C131">
         <v>115</v>
@@ -5565,7 +5565,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C132">
         <v>115</v>
@@ -5576,7 +5576,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C133">
         <v>124</v>
@@ -5587,7 +5587,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C134">
         <v>108</v>
@@ -5598,7 +5598,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C135">
         <v>120</v>
@@ -5609,7 +5609,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C136">
         <v>136</v>
@@ -5620,7 +5620,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C137">
         <v>134</v>
@@ -5631,7 +5631,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C138">
         <v>113</v>
@@ -5642,7 +5642,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C139">
         <v>124</v>
@@ -5653,7 +5653,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>8.2974999999999994</v>
+        <v>46.337500000000006</v>
       </c>
       <c r="C140">
         <v>131</v>
@@ -5664,7 +5664,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C141">
         <v>109</v>
@@ -5675,7 +5675,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C142">
         <v>97</v>
@@ -5686,7 +5686,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C143">
         <v>100</v>
@@ -5697,7 +5697,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C144">
         <v>107</v>
@@ -5708,7 +5708,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C145">
         <v>105</v>
@@ -5719,7 +5719,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C146">
         <v>108</v>
@@ -5730,7 +5730,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C147">
         <v>115</v>
@@ -5741,7 +5741,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C148">
         <v>104</v>
@@ -5752,7 +5752,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C149">
         <v>111</v>
@@ -5763,7 +5763,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C150">
         <v>99</v>
@@ -5774,7 +5774,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C151">
         <v>105</v>
@@ -5785,7 +5785,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C152">
         <v>96</v>
@@ -5796,7 +5796,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C153">
         <v>105</v>
@@ -5807,7 +5807,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C154">
         <v>101</v>
@@ -5818,7 +5818,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C155">
         <v>107</v>
@@ -5829,7 +5829,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C156">
         <v>106</v>
@@ -5840,7 +5840,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C157">
         <v>110</v>
@@ -5851,7 +5851,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C158">
         <v>107</v>
@@ -5862,7 +5862,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C159">
         <v>100</v>
@@ -5873,7 +5873,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C160">
         <v>104</v>
@@ -5884,7 +5884,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C161">
         <v>108</v>
@@ -5895,7 +5895,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C162">
         <v>117</v>
@@ -5906,7 +5906,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C163">
         <v>114</v>
@@ -5917,7 +5917,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C164">
         <v>105</v>
@@ -5928,7 +5928,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C165">
         <v>97</v>
@@ -5939,7 +5939,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C166">
         <v>117</v>
@@ -5950,7 +5950,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C167">
         <v>85</v>
@@ -5961,7 +5961,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C168">
         <v>119</v>
@@ -5972,7 +5972,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C169">
         <v>122</v>
@@ -5983,7 +5983,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C170">
         <v>129</v>
@@ -5994,7 +5994,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C171">
         <v>120</v>
@@ -6005,7 +6005,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C172">
         <v>120</v>
@@ -6016,7 +6016,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C173">
         <v>100</v>
@@ -6027,7 +6027,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C174">
         <v>127</v>
@@ -6038,7 +6038,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C175">
         <v>108</v>
@@ -6049,7 +6049,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>8.2974999999999994</v>
+        <v>0</v>
       </c>
       <c r="C176">
         <v>108</v>
@@ -6060,7 +6060,7 @@
         <v>178</v>
       </c>
       <c r="B177">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C177">
         <v>110</v>
@@ -6071,7 +6071,7 @@
         <v>179</v>
       </c>
       <c r="B178">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C178">
         <v>83</v>
@@ -6082,7 +6082,7 @@
         <v>180</v>
       </c>
       <c r="B179">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C179">
         <v>116</v>
@@ -6093,7 +6093,7 @@
         <v>181</v>
       </c>
       <c r="B180">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C180">
         <v>115</v>
@@ -6104,7 +6104,7 @@
         <v>182</v>
       </c>
       <c r="B181">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C181">
         <v>98</v>
@@ -6115,7 +6115,7 @@
         <v>183</v>
       </c>
       <c r="B182">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C182">
         <v>87</v>
@@ -6126,7 +6126,7 @@
         <v>184</v>
       </c>
       <c r="B183">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C183">
         <v>118</v>
@@ -6137,7 +6137,7 @@
         <v>185</v>
       </c>
       <c r="B184">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C184">
         <v>122</v>
@@ -6148,7 +6148,7 @@
         <v>186</v>
       </c>
       <c r="B185">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C185">
         <v>122</v>
@@ -6159,7 +6159,7 @@
         <v>187</v>
       </c>
       <c r="B186">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C186">
         <v>119</v>
@@ -6170,7 +6170,7 @@
         <v>188</v>
       </c>
       <c r="B187">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C187">
         <v>116</v>
@@ -6181,7 +6181,7 @@
         <v>189</v>
       </c>
       <c r="B188">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C188">
         <v>115</v>
@@ -6192,7 +6192,7 @@
         <v>190</v>
       </c>
       <c r="B189">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C189">
         <v>109</v>
@@ -6203,7 +6203,7 @@
         <v>191</v>
       </c>
       <c r="B190">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C190">
         <v>102</v>
@@ -6214,7 +6214,7 @@
         <v>192</v>
       </c>
       <c r="B191">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C191">
         <v>110</v>
@@ -6225,7 +6225,7 @@
         <v>193</v>
       </c>
       <c r="B192">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C192">
         <v>113</v>
@@ -6236,7 +6236,7 @@
         <v>194</v>
       </c>
       <c r="B193">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C193">
         <v>98</v>
@@ -6247,7 +6247,7 @@
         <v>195</v>
       </c>
       <c r="B194">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C194">
         <v>114</v>
@@ -6258,7 +6258,7 @@
         <v>196</v>
       </c>
       <c r="B195">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C195">
         <v>103</v>
@@ -6269,7 +6269,7 @@
         <v>197</v>
       </c>
       <c r="B196">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C196">
         <v>108</v>
@@ -6280,7 +6280,7 @@
         <v>198</v>
       </c>
       <c r="B197">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C197">
         <v>103</v>
@@ -6291,7 +6291,7 @@
         <v>199</v>
       </c>
       <c r="B198">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C198">
         <v>134</v>
@@ -6302,7 +6302,7 @@
         <v>200</v>
       </c>
       <c r="B199">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="C199">
         <v>107</v>
@@ -6317,7 +6317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -6821,10 +6821,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F577795-8AF9-46CC-BB1D-1353CC91C84D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6836,7 +6836,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>8.4409715080670661E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>0.13311179511974142</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>0.10917302780449024</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>0.11247221879202002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>7.3950997288745213E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>0.18362665928453878</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -6971,8 +6971,12 @@
       <c r="E8">
         <v>8.5549693161343143E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f>D8+D7</f>
+        <v>12.614999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -6988,8 +6992,12 @@
       <c r="E9">
         <v>0.48795491595023388</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" ref="F9:F10" si="0">D9+D8</f>
+        <v>26.442499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -7004,6 +7012,10 @@
       </c>
       <c r="E10">
         <v>0.60383669149862074</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>46.337500000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a new version for the 2nd experiment for lead
</commit_message>
<xml_diff>
--- a/data/lead_data.xlsx
+++ b/data/lead_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhafn\PHY 451\PHY451-GammaRay\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592138E2-FA91-45C9-86DD-E694C1A377EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C205CFB-18BB-4E9A-AEF3-F6C18577BB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24195" yWindow="2775" windowWidth="23595" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28005" yWindow="3885" windowWidth="23595" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lead_v1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="11">
   <si>
     <t>time</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>sigma</t>
+  </si>
+  <si>
+    <t>bg</t>
   </si>
 </sst>
 </file>
@@ -4114,7 +4117,7 @@
   <dimension ref="A1:C199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="M115" sqref="M115"/>
+      <selection activeCell="B141" sqref="B141:B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5663,8 +5666,8 @@
       <c r="A141">
         <v>140</v>
       </c>
-      <c r="B141">
-        <v>0</v>
+      <c r="B141" t="s">
+        <v>10</v>
       </c>
       <c r="C141">
         <v>109</v>
@@ -5674,8 +5677,8 @@
       <c r="A142">
         <v>141</v>
       </c>
-      <c r="B142">
-        <v>0</v>
+      <c r="B142" t="s">
+        <v>10</v>
       </c>
       <c r="C142">
         <v>97</v>
@@ -5685,8 +5688,8 @@
       <c r="A143">
         <v>142</v>
       </c>
-      <c r="B143">
-        <v>0</v>
+      <c r="B143" t="s">
+        <v>10</v>
       </c>
       <c r="C143">
         <v>100</v>
@@ -5696,8 +5699,8 @@
       <c r="A144">
         <v>143</v>
       </c>
-      <c r="B144">
-        <v>0</v>
+      <c r="B144" t="s">
+        <v>10</v>
       </c>
       <c r="C144">
         <v>107</v>
@@ -5707,8 +5710,8 @@
       <c r="A145">
         <v>144</v>
       </c>
-      <c r="B145">
-        <v>0</v>
+      <c r="B145" t="s">
+        <v>10</v>
       </c>
       <c r="C145">
         <v>105</v>
@@ -5718,8 +5721,8 @@
       <c r="A146">
         <v>145</v>
       </c>
-      <c r="B146">
-        <v>0</v>
+      <c r="B146" t="s">
+        <v>10</v>
       </c>
       <c r="C146">
         <v>108</v>
@@ -5729,8 +5732,8 @@
       <c r="A147">
         <v>146</v>
       </c>
-      <c r="B147">
-        <v>0</v>
+      <c r="B147" t="s">
+        <v>10</v>
       </c>
       <c r="C147">
         <v>115</v>
@@ -5740,8 +5743,8 @@
       <c r="A148">
         <v>147</v>
       </c>
-      <c r="B148">
-        <v>0</v>
+      <c r="B148" t="s">
+        <v>10</v>
       </c>
       <c r="C148">
         <v>104</v>
@@ -5751,8 +5754,8 @@
       <c r="A149">
         <v>148</v>
       </c>
-      <c r="B149">
-        <v>0</v>
+      <c r="B149" t="s">
+        <v>10</v>
       </c>
       <c r="C149">
         <v>111</v>
@@ -5762,8 +5765,8 @@
       <c r="A150">
         <v>149</v>
       </c>
-      <c r="B150">
-        <v>0</v>
+      <c r="B150" t="s">
+        <v>10</v>
       </c>
       <c r="C150">
         <v>99</v>
@@ -5773,8 +5776,8 @@
       <c r="A151">
         <v>150</v>
       </c>
-      <c r="B151">
-        <v>0</v>
+      <c r="B151" t="s">
+        <v>10</v>
       </c>
       <c r="C151">
         <v>105</v>
@@ -5784,8 +5787,8 @@
       <c r="A152">
         <v>151</v>
       </c>
-      <c r="B152">
-        <v>0</v>
+      <c r="B152" t="s">
+        <v>10</v>
       </c>
       <c r="C152">
         <v>96</v>
@@ -5795,8 +5798,8 @@
       <c r="A153">
         <v>152</v>
       </c>
-      <c r="B153">
-        <v>0</v>
+      <c r="B153" t="s">
+        <v>10</v>
       </c>
       <c r="C153">
         <v>105</v>
@@ -5806,8 +5809,8 @@
       <c r="A154">
         <v>153</v>
       </c>
-      <c r="B154">
-        <v>0</v>
+      <c r="B154" t="s">
+        <v>10</v>
       </c>
       <c r="C154">
         <v>101</v>
@@ -5817,8 +5820,8 @@
       <c r="A155">
         <v>154</v>
       </c>
-      <c r="B155">
-        <v>0</v>
+      <c r="B155" t="s">
+        <v>10</v>
       </c>
       <c r="C155">
         <v>107</v>
@@ -5828,8 +5831,8 @@
       <c r="A156">
         <v>155</v>
       </c>
-      <c r="B156">
-        <v>0</v>
+      <c r="B156" t="s">
+        <v>10</v>
       </c>
       <c r="C156">
         <v>106</v>
@@ -5839,8 +5842,8 @@
       <c r="A157">
         <v>156</v>
       </c>
-      <c r="B157">
-        <v>0</v>
+      <c r="B157" t="s">
+        <v>10</v>
       </c>
       <c r="C157">
         <v>110</v>
@@ -5850,8 +5853,8 @@
       <c r="A158">
         <v>157</v>
       </c>
-      <c r="B158">
-        <v>0</v>
+      <c r="B158" t="s">
+        <v>10</v>
       </c>
       <c r="C158">
         <v>107</v>
@@ -5861,8 +5864,8 @@
       <c r="A159">
         <v>158</v>
       </c>
-      <c r="B159">
-        <v>0</v>
+      <c r="B159" t="s">
+        <v>10</v>
       </c>
       <c r="C159">
         <v>100</v>
@@ -5872,8 +5875,8 @@
       <c r="A160">
         <v>159</v>
       </c>
-      <c r="B160">
-        <v>0</v>
+      <c r="B160" t="s">
+        <v>10</v>
       </c>
       <c r="C160">
         <v>104</v>
@@ -5883,8 +5886,8 @@
       <c r="A161">
         <v>160</v>
       </c>
-      <c r="B161">
-        <v>0</v>
+      <c r="B161" t="s">
+        <v>10</v>
       </c>
       <c r="C161">
         <v>108</v>
@@ -5894,8 +5897,8 @@
       <c r="A162">
         <v>161</v>
       </c>
-      <c r="B162">
-        <v>0</v>
+      <c r="B162" t="s">
+        <v>10</v>
       </c>
       <c r="C162">
         <v>117</v>
@@ -5905,8 +5908,8 @@
       <c r="A163">
         <v>162</v>
       </c>
-      <c r="B163">
-        <v>0</v>
+      <c r="B163" t="s">
+        <v>10</v>
       </c>
       <c r="C163">
         <v>114</v>
@@ -5916,8 +5919,8 @@
       <c r="A164">
         <v>163</v>
       </c>
-      <c r="B164">
-        <v>0</v>
+      <c r="B164" t="s">
+        <v>10</v>
       </c>
       <c r="C164">
         <v>105</v>
@@ -5927,8 +5930,8 @@
       <c r="A165">
         <v>164</v>
       </c>
-      <c r="B165">
-        <v>0</v>
+      <c r="B165" t="s">
+        <v>10</v>
       </c>
       <c r="C165">
         <v>97</v>
@@ -5938,8 +5941,8 @@
       <c r="A166">
         <v>165</v>
       </c>
-      <c r="B166">
-        <v>0</v>
+      <c r="B166" t="s">
+        <v>10</v>
       </c>
       <c r="C166">
         <v>117</v>
@@ -5949,8 +5952,8 @@
       <c r="A167">
         <v>166</v>
       </c>
-      <c r="B167">
-        <v>0</v>
+      <c r="B167" t="s">
+        <v>10</v>
       </c>
       <c r="C167">
         <v>85</v>
@@ -5960,8 +5963,8 @@
       <c r="A168">
         <v>167</v>
       </c>
-      <c r="B168">
-        <v>0</v>
+      <c r="B168" t="s">
+        <v>10</v>
       </c>
       <c r="C168">
         <v>119</v>
@@ -5971,8 +5974,8 @@
       <c r="A169">
         <v>168</v>
       </c>
-      <c r="B169">
-        <v>0</v>
+      <c r="B169" t="s">
+        <v>10</v>
       </c>
       <c r="C169">
         <v>122</v>
@@ -5982,8 +5985,8 @@
       <c r="A170">
         <v>169</v>
       </c>
-      <c r="B170">
-        <v>0</v>
+      <c r="B170" t="s">
+        <v>10</v>
       </c>
       <c r="C170">
         <v>129</v>
@@ -5993,8 +5996,8 @@
       <c r="A171">
         <v>170</v>
       </c>
-      <c r="B171">
-        <v>0</v>
+      <c r="B171" t="s">
+        <v>10</v>
       </c>
       <c r="C171">
         <v>120</v>
@@ -6004,8 +6007,8 @@
       <c r="A172">
         <v>171</v>
       </c>
-      <c r="B172">
-        <v>0</v>
+      <c r="B172" t="s">
+        <v>10</v>
       </c>
       <c r="C172">
         <v>120</v>
@@ -6015,8 +6018,8 @@
       <c r="A173">
         <v>172</v>
       </c>
-      <c r="B173">
-        <v>0</v>
+      <c r="B173" t="s">
+        <v>10</v>
       </c>
       <c r="C173">
         <v>100</v>
@@ -6026,8 +6029,8 @@
       <c r="A174">
         <v>173</v>
       </c>
-      <c r="B174">
-        <v>0</v>
+      <c r="B174" t="s">
+        <v>10</v>
       </c>
       <c r="C174">
         <v>127</v>
@@ -6037,8 +6040,8 @@
       <c r="A175">
         <v>174</v>
       </c>
-      <c r="B175">
-        <v>0</v>
+      <c r="B175" t="s">
+        <v>10</v>
       </c>
       <c r="C175">
         <v>108</v>
@@ -6048,8 +6051,8 @@
       <c r="A176">
         <v>175</v>
       </c>
-      <c r="B176">
-        <v>0</v>
+      <c r="B176" t="s">
+        <v>10</v>
       </c>
       <c r="C176">
         <v>108</v>
@@ -6059,8 +6062,8 @@
       <c r="A177">
         <v>178</v>
       </c>
-      <c r="B177">
-        <v>0</v>
+      <c r="B177" t="s">
+        <v>10</v>
       </c>
       <c r="C177">
         <v>110</v>
@@ -6070,8 +6073,8 @@
       <c r="A178">
         <v>179</v>
       </c>
-      <c r="B178">
-        <v>0</v>
+      <c r="B178" t="s">
+        <v>10</v>
       </c>
       <c r="C178">
         <v>83</v>
@@ -6081,8 +6084,8 @@
       <c r="A179">
         <v>180</v>
       </c>
-      <c r="B179">
-        <v>0</v>
+      <c r="B179" t="s">
+        <v>10</v>
       </c>
       <c r="C179">
         <v>116</v>
@@ -6092,8 +6095,8 @@
       <c r="A180">
         <v>181</v>
       </c>
-      <c r="B180">
-        <v>0</v>
+      <c r="B180" t="s">
+        <v>10</v>
       </c>
       <c r="C180">
         <v>115</v>
@@ -6103,8 +6106,8 @@
       <c r="A181">
         <v>182</v>
       </c>
-      <c r="B181">
-        <v>0</v>
+      <c r="B181" t="s">
+        <v>10</v>
       </c>
       <c r="C181">
         <v>98</v>
@@ -6114,8 +6117,8 @@
       <c r="A182">
         <v>183</v>
       </c>
-      <c r="B182">
-        <v>0</v>
+      <c r="B182" t="s">
+        <v>10</v>
       </c>
       <c r="C182">
         <v>87</v>
@@ -6125,8 +6128,8 @@
       <c r="A183">
         <v>184</v>
       </c>
-      <c r="B183">
-        <v>0</v>
+      <c r="B183" t="s">
+        <v>10</v>
       </c>
       <c r="C183">
         <v>118</v>
@@ -6136,8 +6139,8 @@
       <c r="A184">
         <v>185</v>
       </c>
-      <c r="B184">
-        <v>0</v>
+      <c r="B184" t="s">
+        <v>10</v>
       </c>
       <c r="C184">
         <v>122</v>
@@ -6147,8 +6150,8 @@
       <c r="A185">
         <v>186</v>
       </c>
-      <c r="B185">
-        <v>0</v>
+      <c r="B185" t="s">
+        <v>10</v>
       </c>
       <c r="C185">
         <v>122</v>
@@ -6158,8 +6161,8 @@
       <c r="A186">
         <v>187</v>
       </c>
-      <c r="B186">
-        <v>0</v>
+      <c r="B186" t="s">
+        <v>10</v>
       </c>
       <c r="C186">
         <v>119</v>
@@ -6169,8 +6172,8 @@
       <c r="A187">
         <v>188</v>
       </c>
-      <c r="B187">
-        <v>0</v>
+      <c r="B187" t="s">
+        <v>10</v>
       </c>
       <c r="C187">
         <v>116</v>
@@ -6180,8 +6183,8 @@
       <c r="A188">
         <v>189</v>
       </c>
-      <c r="B188">
-        <v>0</v>
+      <c r="B188" t="s">
+        <v>10</v>
       </c>
       <c r="C188">
         <v>115</v>
@@ -6191,8 +6194,8 @@
       <c r="A189">
         <v>190</v>
       </c>
-      <c r="B189">
-        <v>0</v>
+      <c r="B189" t="s">
+        <v>10</v>
       </c>
       <c r="C189">
         <v>109</v>
@@ -6202,8 +6205,8 @@
       <c r="A190">
         <v>191</v>
       </c>
-      <c r="B190">
-        <v>0</v>
+      <c r="B190" t="s">
+        <v>10</v>
       </c>
       <c r="C190">
         <v>102</v>
@@ -6213,8 +6216,8 @@
       <c r="A191">
         <v>192</v>
       </c>
-      <c r="B191">
-        <v>0</v>
+      <c r="B191" t="s">
+        <v>10</v>
       </c>
       <c r="C191">
         <v>110</v>
@@ -6224,8 +6227,8 @@
       <c r="A192">
         <v>193</v>
       </c>
-      <c r="B192">
-        <v>0</v>
+      <c r="B192" t="s">
+        <v>10</v>
       </c>
       <c r="C192">
         <v>113</v>
@@ -6235,8 +6238,8 @@
       <c r="A193">
         <v>194</v>
       </c>
-      <c r="B193">
-        <v>0</v>
+      <c r="B193" t="s">
+        <v>10</v>
       </c>
       <c r="C193">
         <v>98</v>
@@ -6246,8 +6249,8 @@
       <c r="A194">
         <v>195</v>
       </c>
-      <c r="B194">
-        <v>0</v>
+      <c r="B194" t="s">
+        <v>10</v>
       </c>
       <c r="C194">
         <v>114</v>
@@ -6257,8 +6260,8 @@
       <c r="A195">
         <v>196</v>
       </c>
-      <c r="B195">
-        <v>0</v>
+      <c r="B195" t="s">
+        <v>10</v>
       </c>
       <c r="C195">
         <v>103</v>
@@ -6268,8 +6271,8 @@
       <c r="A196">
         <v>197</v>
       </c>
-      <c r="B196">
-        <v>0</v>
+      <c r="B196" t="s">
+        <v>10</v>
       </c>
       <c r="C196">
         <v>108</v>
@@ -6279,8 +6282,8 @@
       <c r="A197">
         <v>198</v>
       </c>
-      <c r="B197">
-        <v>0</v>
+      <c r="B197" t="s">
+        <v>10</v>
       </c>
       <c r="C197">
         <v>103</v>
@@ -6290,8 +6293,8 @@
       <c r="A198">
         <v>199</v>
       </c>
-      <c r="B198">
-        <v>0</v>
+      <c r="B198" t="s">
+        <v>10</v>
       </c>
       <c r="C198">
         <v>134</v>
@@ -6301,8 +6304,8 @@
       <c r="A199">
         <v>200</v>
       </c>
-      <c r="B199">
-        <v>0</v>
+      <c r="B199" t="s">
+        <v>10</v>
       </c>
       <c r="C199">
         <v>107</v>

</xml_diff>